<commit_message>
Update May 21 2025
- Updated all Docs, for details see Revision History (new) on last page
- added STEP files in addition to the STL for Transformer parts
- fixed components on Mouser_BOM_for_PCBA despite being already placed on the PCBA, added UCC25600 for PCBA
</commit_message>
<xml_diff>
--- a/kicad/production/DCDCv9-3_Mouser_BOM_for_PCBA.xlsx
+++ b/kicad/production/DCDCv9-3_Mouser_BOM_for_PCBA.xlsx
@@ -11,7 +11,7 @@
     <sheet name="DCDCv9-3_kicad_full_bom" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'DCDCv9-3_kicad_full_bom'!$A$1:$L$49</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'DCDCv9-3_kicad_full_bom'!$A$1:$L$47</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="235">
   <si>
     <t xml:space="preserve">Reference</t>
   </si>
@@ -172,18 +172,6 @@
     <t xml:space="preserve">DCDC-Footprints:C_Disc_D12.5mm_W5.0mm_P10.00mm</t>
   </si>
   <si>
-    <t xml:space="preserve">C5,C33,C46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Taiyo-Yuden/TMK212BBJ106KG-T?qs=PzICbMaShUdwxQxDcETuPw%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TMK212BBJ106KG-T</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DCDC-Footprints:C_0805_2012Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">D1</t>
   </si>
   <si>
@@ -212,18 +200,6 @@
   </si>
   <si>
     <t xml:space="preserve">DCDC-Footprints:D_SMF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D3,D4,D5,D6,D7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.mouser.de/ProductDetail/Inolux/IN-S63AT5G?qs=fAHHVMwC%252Bbiw6WrSEma0zA%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IN-S63AT5G</t>
   </si>
   <si>
     <t xml:space="preserve">F1</t>
@@ -975,10 +951,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+      <selection pane="topLeft" activeCell="A43" activeCellId="0" sqref="43:43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1234,19 +1210,19 @@
         <v>49</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F9" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I9" s="1" t="n">
         <v>1</v>
@@ -1257,24 +1233,24 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1" t="n">
         <v>1</v>
       </c>
       <c r="L10" s="1" t="s">
@@ -1283,25 +1259,28 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>17</v>
@@ -1309,25 +1288,22 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>17</v>
@@ -1335,28 +1311,25 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F13" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>17</v>
@@ -1364,22 +1337,28 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="F14" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>17</v>
@@ -1387,25 +1366,28 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="F15" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H15" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>17</v>
@@ -1413,19 +1395,19 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F16" s="1" t="n">
         <v>1</v>
@@ -1433,8 +1415,11 @@
       <c r="H16" s="1" t="n">
         <v>1</v>
       </c>
+      <c r="J16" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="K16" s="1" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>17</v>
@@ -1442,28 +1427,31 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K17" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="F17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>93</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>17</v>
@@ -1471,31 +1459,25 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="L18" s="1" t="s">
         <v>17</v>
@@ -1503,19 +1485,19 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>74</v>
+        <v>104</v>
       </c>
       <c r="F19" s="1" t="n">
         <v>1</v>
@@ -1523,11 +1505,8 @@
       <c r="H19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="K19" s="1" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="L19" s="1" t="s">
         <v>17</v>
@@ -1535,25 +1514,28 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1" t="n">
         <v>1</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>109</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>17</v>
@@ -1561,45 +1543,42 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="F21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H21" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="L21" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>116</v>
+        <v>66</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>118</v>
       </c>
       <c r="F22" s="1" t="n">
         <v>1</v>
@@ -1607,127 +1586,130 @@
       <c r="H22" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J22" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="K22" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>124</v>
+        <v>96</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>125</v>
+        <v>97</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="F24" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="H24" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>127</v>
+      <c r="I24" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="L25" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="L25" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D26" s="1" t="s">
-        <v>106</v>
+        <v>134</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="F26" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H26" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I26" s="1" t="n">
-        <v>1</v>
+      <c r="J26" s="1" t="s">
+        <v>136</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>17</v>
@@ -1735,19 +1717,19 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>74</v>
+        <v>139</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <v>7443091100</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="F27" s="1" t="n">
         <v>1</v>
@@ -1755,28 +1737,25 @@
       <c r="H27" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K27" s="1" t="s">
-        <v>137</v>
-      </c>
       <c r="L27" s="1" t="s">
-        <v>138</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>1</v>
@@ -1785,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>17</v>
@@ -1793,28 +1772,28 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J29" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="1" t="n">
-        <v>7443091100</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H29" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="L29" s="1" t="s">
-        <v>17</v>
+        <v>120</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1828,19 +1807,16 @@
         <v>151</v>
       </c>
       <c r="D30" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E30" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="F30" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>17</v>
@@ -1848,28 +1824,28 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="F31" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J31" s="1" t="s">
-        <v>155</v>
+      <c r="H31" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>128</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1886,10 +1862,10 @@
         <v>158</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F32" s="1" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1" t="n">
         <v>1</v>
@@ -1900,16 +1876,16 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="D33" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>162</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>164</v>
@@ -1917,8 +1893,11 @@
       <c r="F33" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H33" s="1" t="n">
-        <v>1</v>
+      <c r="I33" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>165</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>17</v>
@@ -1926,25 +1905,28 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>164</v>
+        <v>170</v>
       </c>
       <c r="F34" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H34" s="1" t="n">
-        <v>1</v>
+      <c r="I34" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>17</v>
@@ -1952,28 +1934,28 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F35" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I35" s="1" t="n">
+      <c r="H35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>17</v>
@@ -1981,28 +1963,31 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="E36" s="1" t="s">
-        <v>178</v>
+        <v>66</v>
       </c>
       <c r="F36" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I36" s="1" t="n">
-        <v>1</v>
+      <c r="H36" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L36" s="1" t="s">
         <v>17</v>
@@ -2010,28 +1995,31 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J37" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="F37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H37" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="K37" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L37" s="1" t="s">
         <v>17</v>
@@ -2048,132 +2036,126 @@
         <v>188</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="F38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H38" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="J38" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>17</v>
+        <v>192</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="K39" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="L39" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F39" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H39" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J39" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="L39" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>74</v>
+        <v>99</v>
       </c>
       <c r="F40" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J40" s="1" t="s">
-        <v>198</v>
+      <c r="H40" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>199</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="D41" s="1" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>74</v>
+        <v>204</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J41" s="1" t="s">
-        <v>198</v>
+        <v>1</v>
+      </c>
+      <c r="H41" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="L41" s="1" t="s">
-        <v>200</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>107</v>
+        <v>209</v>
       </c>
       <c r="F42" s="1" t="n">
         <v>1</v>
@@ -2181,8 +2163,8 @@
       <c r="H42" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="K42" s="1" t="s">
-        <v>207</v>
+      <c r="J42" s="1" t="s">
+        <v>210</v>
       </c>
       <c r="L42" s="1" t="s">
         <v>17</v>
@@ -2190,28 +2172,28 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F43" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H43" s="1" t="n">
+      <c r="I43" s="1" t="n">
         <v>1</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="L43" s="1" t="s">
         <v>17</v>
@@ -2219,19 +2201,19 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F44" s="1" t="n">
         <v>1</v>
@@ -2239,8 +2221,8 @@
       <c r="H44" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>218</v>
+      <c r="K44" s="1" t="s">
+        <v>221</v>
       </c>
       <c r="L44" s="1" t="s">
         <v>17</v>
@@ -2248,28 +2230,28 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>223</v>
-      </c>
       <c r="F45" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I45" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>224</v>
+      <c r="H45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>225</v>
       </c>
       <c r="L45" s="1" t="s">
         <v>17</v>
@@ -2277,28 +2259,25 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="F46" s="1" t="n">
         <v>1</v>
       </c>
       <c r="H46" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="L46" s="1" t="s">
         <v>17</v>
@@ -2306,87 +2285,32 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="E47" s="1" t="s">
-        <v>228</v>
+        <v>234</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H47" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>233</v>
-      </c>
       <c r="L47" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F48" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H48" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="F49" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="H49" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="L49" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L49"/>
+  <autoFilter ref="A1:L47"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>